<commit_message>
updated notebook and datasets
</commit_message>
<xml_diff>
--- a/notebook/provsvar_tabel.xlsx
+++ b/notebook/provsvar_tabel.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -44,6 +44,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -65,12 +70,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -542,11 +548,11 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>8201113167</v>
+        <v>8201113194</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9-12-2021</t>
+          <t>30/11/2021</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -555,7 +561,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
@@ -568,7 +574,7 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
@@ -581,7 +587,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="L2" s="2" t="inlineStr">
         <is>
@@ -594,7 +600,7 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>0.33</v>
+        <v>0.39</v>
       </c>
       <c r="O2" s="2" t="inlineStr">
         <is>
@@ -607,29 +613,29 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0.16</v>
+        <v>0.34</v>
       </c>
       <c r="R2" s="2" t="inlineStr">
         <is>
           <t>GRON</t>
         </is>
       </c>
-      <c r="S2" s="2" t="inlineStr">
-        <is>
-          <t>GRON</t>
+      <c r="S2" s="3" t="inlineStr">
+        <is>
+          <t>RÖD</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B3" t="n">
-        <v>8201113170</v>
+        <v>8201113197</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8-12-2021</t>
+          <t>29/11/2021</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -638,7 +644,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
@@ -647,11 +653,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>T3, fritt, P-</t>
+          <t>T3, P-</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>3.3</v>
+        <v>0.87</v>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
@@ -664,11 +670,11 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>GRON</t>
+        <v>6.4</v>
+      </c>
+      <c r="L3" s="4" t="inlineStr">
+        <is>
+          <t>GUL</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -677,7 +683,7 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>0.26</v>
+        <v>0.52</v>
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
@@ -690,11 +696,11 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="R3" s="3" t="inlineStr">
-        <is>
-          <t>GUL</t>
+        <v>0.48</v>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>GRON</t>
         </is>
       </c>
       <c r="S3" s="2" t="inlineStr">
@@ -705,14 +711,14 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B4" t="n">
-        <v>8201113173</v>
+        <v>8201113206</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7-12-2021</t>
+          <t>26/11/2021</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -721,7 +727,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
@@ -730,11 +736,11 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>T3, fritt, P-</t>
+          <t>T3, P-</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>4.2</v>
+        <v>1.2</v>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
@@ -760,7 +766,7 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>0.71</v>
+        <v>0.4</v>
       </c>
       <c r="O4" s="2" t="inlineStr">
         <is>
@@ -773,7 +779,7 @@
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>0.58</v>
+        <v>0.18</v>
       </c>
       <c r="R4" s="2" t="inlineStr">
         <is>

</xml_diff>